<commit_message>
updated python and expanded livestock elasticities to include all categories to drop category switching
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/india/model_input_variables_india_ce_calibrated.xlsx
+++ b/ref/ingestion/calibrated/india/model_input_variables_india_ce_calibrated.xlsx
@@ -20794,7 +20794,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
@@ -20987,7 +20987,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
@@ -21180,7 +21180,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
@@ -21373,7 +21373,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
@@ -21566,7 +21566,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
@@ -21759,7 +21759,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
@@ -21952,7 +21952,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
@@ -22145,7 +22145,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
@@ -22338,7 +22338,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
@@ -22531,7 +22531,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
@@ -22724,7 +22724,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
@@ -22917,7 +22917,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
@@ -23110,7 +23110,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
@@ -23303,7 +23303,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
@@ -23496,7 +23496,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
@@ -23689,7 +23689,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
@@ -23882,7 +23882,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
@@ -24075,7 +24075,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
@@ -24268,7 +24268,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
@@ -24461,7 +24461,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr"/>
@@ -24654,7 +24654,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr"/>
@@ -24847,7 +24847,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr"/>
@@ -25040,7 +25040,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
@@ -25233,7 +25233,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
@@ -25426,7 +25426,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
@@ -25619,7 +25619,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
@@ -52075,139 +52075,139 @@
         <v>0</v>
       </c>
       <c r="U6" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V6" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W6" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X6" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK6" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR6" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS6" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT6" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV6" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW6" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX6" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY6" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ6" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA6" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB6" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC6" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD6" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE6" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF6" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK6" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL6" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM6" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="7">
@@ -52268,139 +52268,139 @@
         <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V7" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W7" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X7" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL7" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM7" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN7" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ7" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR7" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS7" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT7" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU7" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV7" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW7" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX7" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY7" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ7" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA7" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB7" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC7" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD7" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE7" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF7" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG7" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH7" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI7" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ7" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK7" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL7" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM7" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8">
@@ -52461,139 +52461,139 @@
         <v>0</v>
       </c>
       <c r="U8" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V8" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W8" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X8" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH8" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI8" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK8" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL8" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM8" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN8" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ8" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR8" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS8" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT8" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW8" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX8" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY8" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ8" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA8" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB8" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC8" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD8" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE8" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF8" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH8" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK8" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL8" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM8" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9">
@@ -52654,139 +52654,139 @@
         <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V9" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W9" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X9" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH9" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI9" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK9" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL9" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM9" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN9" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS9" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV9" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW9" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX9" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY9" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ9" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA9" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB9" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC9" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD9" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE9" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF9" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG9" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH9" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK9" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL9" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM9" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -60606,139 +60606,139 @@
         <v>0</v>
       </c>
       <c r="U41" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V41" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W41" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X41" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y41" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z41" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA41" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB41" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC41" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD41" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE41" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF41" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG41" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH41" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI41" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ41" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK41" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL41" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM41" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN41" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO41" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP41" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ41" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR41" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS41" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT41" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU41" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV41" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW41" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX41" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY41" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ41" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA41" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB41" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC41" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD41" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE41" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF41" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG41" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH41" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI41" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ41" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK41" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL41" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM41" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="42">
@@ -60799,139 +60799,139 @@
         <v>0</v>
       </c>
       <c r="U42" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V42" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W42" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X42" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y42" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z42" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA42" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB42" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC42" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD42" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE42" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF42" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG42" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH42" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI42" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ42" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK42" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL42" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM42" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN42" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO42" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP42" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ42" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR42" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS42" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT42" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU42" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV42" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW42" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX42" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY42" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ42" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA42" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB42" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC42" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD42" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE42" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF42" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG42" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH42" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI42" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ42" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK42" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL42" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM42" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="43">
@@ -60992,139 +60992,139 @@
         <v>0</v>
       </c>
       <c r="U43" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V43" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W43" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X43" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y43" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z43" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA43" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB43" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC43" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD43" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE43" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF43" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG43" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH43" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI43" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ43" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK43" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL43" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM43" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN43" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO43" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP43" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ43" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR43" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS43" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT43" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU43" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV43" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW43" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX43" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY43" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ43" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA43" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB43" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC43" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD43" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE43" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF43" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG43" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH43" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI43" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ43" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK43" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL43" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM43" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="44">
@@ -61185,139 +61185,139 @@
         <v>0</v>
       </c>
       <c r="U44" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V44" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W44" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X44" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y44" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z44" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA44" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB44" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC44" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD44" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE44" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF44" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG44" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH44" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI44" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ44" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK44" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL44" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM44" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN44" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO44" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP44" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ44" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR44" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS44" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT44" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU44" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV44" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW44" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX44" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY44" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ44" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA44" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB44" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC44" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD44" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE44" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF44" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG44" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH44" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI44" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ44" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK44" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL44" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM44" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
@@ -69137,139 +69137,139 @@
         <v>0</v>
       </c>
       <c r="U41" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V41" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W41" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X41" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y41" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z41" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA41" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB41" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC41" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD41" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE41" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF41" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG41" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH41" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI41" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ41" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK41" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL41" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM41" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN41" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO41" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP41" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ41" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR41" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS41" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT41" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU41" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV41" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW41" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX41" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY41" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ41" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA41" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB41" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC41" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD41" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE41" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF41" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG41" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH41" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI41" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ41" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK41" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL41" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM41" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="42">
@@ -69330,139 +69330,139 @@
         <v>0</v>
       </c>
       <c r="U42" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V42" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W42" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X42" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y42" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z42" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA42" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB42" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC42" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD42" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE42" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF42" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG42" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH42" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI42" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ42" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK42" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL42" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM42" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN42" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO42" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP42" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ42" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR42" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS42" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT42" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU42" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV42" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW42" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX42" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY42" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ42" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA42" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB42" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC42" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD42" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE42" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF42" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG42" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH42" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI42" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ42" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK42" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL42" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM42" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="43">
@@ -69523,139 +69523,139 @@
         <v>0</v>
       </c>
       <c r="U43" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V43" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W43" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X43" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y43" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z43" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA43" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB43" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC43" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD43" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE43" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF43" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG43" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH43" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI43" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ43" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK43" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL43" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM43" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN43" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO43" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP43" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ43" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR43" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS43" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT43" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU43" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV43" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW43" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX43" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY43" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ43" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA43" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB43" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC43" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD43" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE43" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF43" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG43" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH43" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI43" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ43" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK43" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL43" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM43" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="44">
@@ -69716,139 +69716,139 @@
         <v>0</v>
       </c>
       <c r="U44" t="n">
-        <v>0.01888888888888889</v>
+        <v>0.02</v>
       </c>
       <c r="V44" t="n">
-        <v>0.03777777777777778</v>
+        <v>0.04</v>
       </c>
       <c r="W44" t="n">
-        <v>0.05666666666666666</v>
+        <v>0.06</v>
       </c>
       <c r="X44" t="n">
-        <v>0.07555555555555556</v>
+        <v>0.08</v>
       </c>
       <c r="Y44" t="n">
-        <v>0.09444444444444444</v>
+        <v>0.09999999999999999</v>
       </c>
       <c r="Z44" t="n">
-        <v>0.1133333333333333</v>
+        <v>0.12</v>
       </c>
       <c r="AA44" t="n">
-        <v>0.1322222222222222</v>
+        <v>0.14</v>
       </c>
       <c r="AB44" t="n">
-        <v>0.1511111111111111</v>
+        <v>0.16</v>
       </c>
       <c r="AC44" t="n">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="AD44" t="n">
-        <v>0.1888888888888889</v>
+        <v>0.2</v>
       </c>
       <c r="AE44" t="n">
-        <v>0.2077777777777778</v>
+        <v>0.22</v>
       </c>
       <c r="AF44" t="n">
-        <v>0.2266666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="AG44" t="n">
-        <v>0.2455555555555555</v>
+        <v>0.26</v>
       </c>
       <c r="AH44" t="n">
-        <v>0.2644444444444444</v>
+        <v>0.28</v>
       </c>
       <c r="AI44" t="n">
-        <v>0.2833333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="AJ44" t="n">
-        <v>0.3022222222222222</v>
+        <v>0.32</v>
       </c>
       <c r="AK44" t="n">
-        <v>0.3211111111111111</v>
+        <v>0.34</v>
       </c>
       <c r="AL44" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="AM44" t="n">
-        <v>0.3588888888888889</v>
+        <v>0.38</v>
       </c>
       <c r="AN44" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.4</v>
       </c>
       <c r="AO44" t="n">
-        <v>0.3966666666666667</v>
+        <v>0.42</v>
       </c>
       <c r="AP44" t="n">
-        <v>0.4155555555555555</v>
+        <v>0.44</v>
       </c>
       <c r="AQ44" t="n">
-        <v>0.4344444444444444</v>
+        <v>0.46</v>
       </c>
       <c r="AR44" t="n">
-        <v>0.4533333333333333</v>
+        <v>0.48</v>
       </c>
       <c r="AS44" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="AT44" t="n">
-        <v>0.4911111111111111</v>
+        <v>0.52</v>
       </c>
       <c r="AU44" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
       <c r="AV44" t="n">
-        <v>0.5288888888888889</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AW44" t="n">
-        <v>0.5477777777777778</v>
+        <v>0.5800000000000001</v>
       </c>
       <c r="AX44" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.6</v>
       </c>
       <c r="AY44" t="n">
-        <v>0.5855555555555555</v>
+        <v>0.62</v>
       </c>
       <c r="AZ44" t="n">
-        <v>0.6044444444444445</v>
+        <v>0.64</v>
       </c>
       <c r="BA44" t="n">
-        <v>0.6233333333333333</v>
+        <v>0.6599999999999999</v>
       </c>
       <c r="BB44" t="n">
-        <v>0.6422222222222221</v>
+        <v>0.68</v>
       </c>
       <c r="BC44" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.7000000000000001</v>
       </c>
       <c r="BD44" t="n">
-        <v>0.68</v>
+        <v>0.7200000000000001</v>
       </c>
       <c r="BE44" t="n">
-        <v>0.6988888888888889</v>
+        <v>0.74</v>
       </c>
       <c r="BF44" t="n">
-        <v>0.7177777777777777</v>
+        <v>0.76</v>
       </c>
       <c r="BG44" t="n">
-        <v>0.7366666666666667</v>
+        <v>0.78</v>
       </c>
       <c r="BH44" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="BI44" t="n">
-        <v>0.7744444444444444</v>
+        <v>0.82</v>
       </c>
       <c r="BJ44" t="n">
-        <v>0.7933333333333333</v>
+        <v>0.8400000000000001</v>
       </c>
       <c r="BK44" t="n">
-        <v>0.8122222222222223</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="BL44" t="n">
-        <v>0.831111111111111</v>
+        <v>0.88</v>
       </c>
       <c r="BM44" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>